<commit_message>
Updated default value for UI settings in FA_all.py, added new binary text files for analysis, and modified existing batch results files.
</commit_message>
<xml_diff>
--- a/saved_data/batch_results_n=1,split=word,condition=no,definition=static,min_dist=1,overlap=overlapping.xlsx
+++ b/saved_data/batch_results_n=1,split=word,condition=no,definition=static,min_dist=1,overlap=overlapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,26 @@
           <t>dgw</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>w_val</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>wh_val</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>we_val</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>wm_val</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -511,44 +531,56 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hobbit_en.txt</t>
+          <t>Akuma.txt</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>99</v>
       </c>
       <c r="D2" t="n">
-        <v>95384</v>
+        <v>195</v>
       </c>
       <c r="E2" t="n">
-        <v>6483</v>
+        <v>196</v>
       </c>
       <c r="F2" t="n">
-        <v>1.8139</v>
+        <v>5.199</v>
       </c>
       <c r="G2" t="n">
-        <v>1.29707863</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.42560607</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>1.2359205</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.34504063</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4705261</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.15071457</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.47315779</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0.16769265</v>
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>9</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -557,44 +589,56 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Clarke, Arthur C - Cradle.txt</t>
+          <t>+The jungle book_Kipling.txt</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>204</v>
+        <v>123</v>
       </c>
       <c r="D3" t="n">
-        <v>140001</v>
+        <v>12869</v>
       </c>
       <c r="E3" t="n">
-        <v>10624</v>
+        <v>1968</v>
       </c>
       <c r="F3" t="n">
-        <v>1.6408</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>1.47802178</v>
+        <v>1.1098079</v>
       </c>
       <c r="H3" t="n">
-        <v>0.79717105</v>
+        <v>0.27415415</v>
       </c>
       <c r="I3" t="n">
-        <v>1.45596446</v>
+        <v>1.07519404</v>
       </c>
       <c r="J3" t="n">
-        <v>0.77980818</v>
+        <v>0.23230313</v>
       </c>
       <c r="K3" t="n">
-        <v>0.47775085</v>
+        <v>0.56357167</v>
       </c>
       <c r="L3" t="n">
-        <v>0.13169218</v>
+        <v>0.08426578</v>
       </c>
       <c r="M3" t="n">
-        <v>0.48473192</v>
+        <v>0.57244588</v>
       </c>
       <c r="N3" t="n">
-        <v>0.11633351</v>
+        <v>0.07031314</v>
+      </c>
+      <c r="O3" t="n">
+        <v>640</v>
+      </c>
+      <c r="P3" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>32</v>
+      </c>
+      <c r="R3" t="n">
+        <v>643</v>
       </c>
     </row>
     <row r="4">
@@ -603,44 +647,56 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Don_Quixote06w.txt</t>
+          <t>abusaeed_norm.txt</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>344</v>
+        <v>140</v>
       </c>
       <c r="D4" t="n">
-        <v>200005</v>
+        <v>21761</v>
       </c>
       <c r="E4" t="n">
-        <v>10062</v>
+        <v>4535</v>
       </c>
       <c r="F4" t="n">
-        <v>2.4622</v>
+        <v>0.1621</v>
       </c>
       <c r="G4" t="n">
-        <v>1.28287416</v>
+        <v>1.31420119</v>
       </c>
       <c r="H4" t="n">
-        <v>0.31949285</v>
+        <v>0.21865455</v>
       </c>
       <c r="I4" t="n">
-        <v>1.21797637</v>
+        <v>1.27099541</v>
       </c>
       <c r="J4" t="n">
-        <v>0.30005378</v>
+        <v>0.1871897</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4666401</v>
+        <v>0.5981702</v>
       </c>
       <c r="L4" t="n">
-        <v>0.09384217</v>
+        <v>0.08834663</v>
       </c>
       <c r="M4" t="n">
-        <v>0.46068725</v>
+        <v>0.6116636600000001</v>
       </c>
       <c r="N4" t="n">
-        <v>0.08994765</v>
+        <v>0.0839739</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1080</v>
+      </c>
+      <c r="P4" t="n">
+        <v>54</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>54</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1088</v>
       </c>
     </row>
     <row r="5">
@@ -649,140 +705,640 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>++1VMS_freie.txt</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>168</v>
+      </c>
+      <c r="D5" t="n">
+        <v>37023</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8493</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.88285554</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.56093097</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.85963486</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.52967209</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.76796855</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.07331263</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.7821254</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.07088313</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1840</v>
+      </c>
+      <c r="P5" t="n">
+        <v>92</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>92</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>serbian_èá¼Ñ¡« ñ«íá_space&amp;paragraph.txt</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>167</v>
+      </c>
+      <c r="D6" t="n">
+        <v>36206</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8743</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.16267184</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.12293302</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.1320443</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.10882921</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.59203826</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.09637063</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.61673956</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.09186859999999999</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1800</v>
+      </c>
+      <c r="P6" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>90</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>serbian_èá¼Ñ¡« ñ«íá.txt</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>167</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36206</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8743</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3545</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.16267184</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.12293302</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.1320443</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.10882921</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.59203826</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.09637063</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.61673956</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.09186859999999999</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1800</v>
+      </c>
+      <c r="P7" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>90</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Hobbit_en.txt</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>278</v>
+      </c>
+      <c r="D8" t="n">
+        <v>95384</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6483</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.7828000000000001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.27116996</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.27468998</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.2149969</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.27959935</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.5979452200000001</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.08562182</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.62898307</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.09219381</v>
+      </c>
+      <c r="O8" t="n">
+        <v>4760</v>
+      </c>
+      <c r="P8" t="n">
+        <v>238</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>238</v>
+      </c>
+      <c r="R8" t="n">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Robinson_Crusoe.txt</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>326</v>
+      </c>
+      <c r="D9" t="n">
+        <v>121082</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6178</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.0059</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.36132809</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.60820567</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.26246773</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.50276359</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.60539885</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.12348999</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.61949932</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.12069688</v>
+      </c>
+      <c r="O9" t="n">
+        <v>6040</v>
+      </c>
+      <c r="P9" t="n">
+        <v>302</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>302</v>
+      </c>
+      <c r="R9" t="n">
+        <v>6054</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Clarke, Arthur C - Cradle.txt</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>362</v>
+      </c>
+      <c r="D10" t="n">
+        <v>140001</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10624</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.4981</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.5353913</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.83732996</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.46293596</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.78323261</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.58122398</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.08165206999999999</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.60020894</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.08190675</v>
+      </c>
+      <c r="O10" t="n">
+        <v>6650</v>
+      </c>
+      <c r="P10" t="n">
+        <v>350</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>350</v>
+      </c>
+      <c r="R10" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Don_Quixote06w.txt</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>474</v>
+      </c>
+      <c r="D11" t="n">
+        <v>200005</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10062</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.9388</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.30696882</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.34847381</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.21897882</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.30692816</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.50859979</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.06579174</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.51552494</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.06097659</v>
+      </c>
+      <c r="O11" t="n">
+        <v>9500</v>
+      </c>
+      <c r="P11" t="n">
+        <v>500</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>500</v>
+      </c>
+      <c r="R11" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>+monkey_text_M5k_L1kk.txt</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>388</v>
+      </c>
+      <c r="D12" t="n">
+        <v>153795</v>
+      </c>
+      <c r="E12" t="n">
+        <v>124250</v>
+      </c>
+      <c r="F12" t="n">
+        <v>22.2234</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>7680</v>
+      </c>
+      <c r="P12" t="n">
+        <v>384</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>384</v>
+      </c>
+      <c r="R12" t="n">
+        <v>7689</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>LOTR_en.txt</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C13" t="n">
         <v>999</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D13" t="n">
         <v>479149</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E13" t="n">
         <v>14261</v>
       </c>
-      <c r="F5" t="n">
-        <v>5.4605</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="F13" t="n">
+        <v>10.5303</v>
+      </c>
+      <c r="G13" t="n">
         <v>1.45826326</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H13" t="n">
         <v>0.7575868</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I13" t="n">
         <v>1.34609843</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J13" t="n">
         <v>0.56788795</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K13" t="n">
         <v>0.62062058</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L13" t="n">
         <v>0.08035713</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M13" t="n">
         <v>0.64061024</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N13" t="n">
         <v>0.0766343</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="O13" t="n">
+        <v>23940</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1197</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1197</v>
+      </c>
+      <c r="R13" t="n">
+        <v>23957</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>411.5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>228634.75</v>
-      </c>
-      <c r="E6" t="n">
-        <v>10357.5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2.84435</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.37905946</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.57496419</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.31398994</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.49819764</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.50888441</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.11415151</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.5147968000000001</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.11265203</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="C14" t="n">
+        <v>307.58333333</v>
+      </c>
+      <c r="D14" t="n">
+        <v>111139.66666667</v>
+      </c>
+      <c r="E14" t="n">
+        <v>17044.66666667</v>
+      </c>
+      <c r="F14" t="n">
+        <v>3.71395833</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.13044414</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.34382433</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.08128256</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.30060292</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.50229795</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.07296492</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.51704505</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.07010964</v>
+      </c>
+      <c r="O14" t="n">
+        <v>5478.25</v>
+      </c>
+      <c r="P14" t="n">
+        <v>277.5</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>277.5</v>
+      </c>
+      <c r="R14" t="n">
+        <v>5556.75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>StdDev</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Std. Dev.</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>350.15175282</v>
-      </c>
-      <c r="D7" t="n">
-        <v>149322.43305407</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2757.14548945</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.54115535</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.08949756</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.20633732</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.09552639</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.19162417</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.06463399</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.02828012</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.07313441</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.03484175</v>
+      <c r="C15" t="n">
+        <v>238.23428886</v>
+      </c>
+      <c r="D15" t="n">
+        <v>126821.80413828</v>
+      </c>
+      <c r="E15" t="n">
+        <v>32530.74146694</v>
+      </c>
+      <c r="F15" t="n">
+        <v>6.28740705</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.54267242</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.2725067</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.52208017</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.23629104</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.23171236</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.03535815</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.23840662</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.0344993</v>
+      </c>
+      <c r="O15" t="n">
+        <v>6304.92336888</v>
+      </c>
+      <c r="P15" t="n">
+        <v>316.90469125</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>316.90469125</v>
+      </c>
+      <c r="R15" t="n">
+        <v>6340.99686071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored file upload status handling in FA_all.py to use console logging for success and error messages, and added a summary display for upload results. Updated Flask server to listen on all interfaces.
</commit_message>
<xml_diff>
--- a/saved_data/batch_results_n=1,split=word,condition=no,definition=static,min_dist=1,overlap=overlapping.xlsx
+++ b/saved_data/batch_results_n=1,split=word,condition=no,definition=static,min_dist=1,overlap=overlapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,56 +531,56 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hobbit_en.txt</t>
+          <t>++1VMS_freie.txt</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>219</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>95384</v>
+        <v>37023</v>
       </c>
       <c r="E2" t="n">
-        <v>6483</v>
+        <v>8493</v>
       </c>
       <c r="F2" t="n">
-        <v>1.0099</v>
+        <v>5.8571</v>
       </c>
       <c r="G2" t="n">
-        <v>1.26099702</v>
+        <v>1.12207639</v>
       </c>
       <c r="H2" t="n">
-        <v>0.28156947</v>
+        <v>0.46400344</v>
       </c>
       <c r="I2" t="n">
-        <v>1.21484827</v>
+        <v>1.54206235</v>
       </c>
       <c r="J2" t="n">
-        <v>0.28070574</v>
+        <v>0.54920379</v>
       </c>
       <c r="K2" t="n">
-        <v>0.58881766</v>
+        <v>0.55756473</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08579006</v>
+        <v>0.09580913000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>0.62415326</v>
+        <v>0.66171355</v>
       </c>
       <c r="N2" t="n">
-        <v>0.09317209999999999</v>
+        <v>0.12229434</v>
       </c>
       <c r="O2" t="n">
-        <v>4760</v>
+        <v>1840</v>
       </c>
       <c r="P2" t="n">
-        <v>238</v>
+        <v>92</v>
       </c>
       <c r="Q2" t="n">
-        <v>238</v>
+        <v>92</v>
       </c>
       <c r="R2" t="n">
-        <v>4769</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="3">
@@ -589,56 +589,56 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Clarke, Arthur C - Cradle.txt</t>
+          <t>+The jungle book_Kipling.txt</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>310</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>140001</v>
+        <v>12869</v>
       </c>
       <c r="E3" t="n">
-        <v>10624</v>
+        <v>1968</v>
       </c>
       <c r="F3" t="n">
-        <v>1.4915</v>
+        <v>0.8956</v>
       </c>
       <c r="G3" t="n">
-        <v>1.5717537</v>
+        <v>1.0191548</v>
       </c>
       <c r="H3" t="n">
-        <v>0.90740088</v>
+        <v>0.36221641</v>
       </c>
       <c r="I3" t="n">
-        <v>1.47559508</v>
+        <v>1.12898535</v>
       </c>
       <c r="J3" t="n">
-        <v>0.80767773</v>
+        <v>0.34096765</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5958764</v>
+        <v>0.53407091</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08239866999999999</v>
+        <v>0.08525067</v>
       </c>
       <c r="M3" t="n">
-        <v>0.6251047</v>
+        <v>0.56538152</v>
       </c>
       <c r="N3" t="n">
-        <v>0.08623585</v>
+        <v>0.09295657</v>
       </c>
       <c r="O3" t="n">
-        <v>4760</v>
+        <v>640</v>
       </c>
       <c r="P3" t="n">
-        <v>238</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="n">
-        <v>238</v>
+        <v>32</v>
       </c>
       <c r="R3" t="n">
-        <v>4769</v>
+        <v>643</v>
       </c>
     </row>
     <row r="4">
@@ -647,56 +647,56 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Don_Quixote06w.txt</t>
+          <t>abusaeed_norm.txt</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>432</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>200005</v>
+        <v>21761</v>
       </c>
       <c r="E4" t="n">
-        <v>10062</v>
+        <v>4535</v>
       </c>
       <c r="F4" t="n">
-        <v>2.0115</v>
+        <v>1.9969</v>
       </c>
       <c r="G4" t="n">
-        <v>1.3067195</v>
+        <v>1.07212801</v>
       </c>
       <c r="H4" t="n">
-        <v>0.34056569</v>
+        <v>0.45418254</v>
       </c>
       <c r="I4" t="n">
-        <v>1.22050053</v>
+        <v>1.23386683</v>
       </c>
       <c r="J4" t="n">
-        <v>0.30551673</v>
+        <v>0.37706908</v>
       </c>
       <c r="K4" t="n">
-        <v>0.52596456</v>
+        <v>0.50640681</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0450144</v>
+        <v>0.06523311</v>
       </c>
       <c r="M4" t="n">
-        <v>0.53412594</v>
+        <v>0.54894024</v>
       </c>
       <c r="N4" t="n">
-        <v>0.05055469</v>
+        <v>0.08749202</v>
       </c>
       <c r="O4" t="n">
-        <v>4760</v>
+        <v>1080</v>
       </c>
       <c r="P4" t="n">
-        <v>238</v>
+        <v>54</v>
       </c>
       <c r="Q4" t="n">
-        <v>238</v>
+        <v>54</v>
       </c>
       <c r="R4" t="n">
-        <v>4769</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="5">
@@ -705,56 +705,56 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>serbian_èá¼Ñ¡« ñ«íá.txt</t>
+          <t>Akuma.txt</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>36206</v>
+        <v>195</v>
       </c>
       <c r="E5" t="n">
-        <v>8743</v>
+        <v>196</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3734</v>
+        <v>0.0247</v>
       </c>
       <c r="G5" t="n">
-        <v>1.22048166</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.30377293</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1.15587978</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.19893013</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.51418123</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1234539</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.52967164</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0.14762075</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>4760</v>
+        <v>9</v>
       </c>
       <c r="P5" t="n">
-        <v>238</v>
+        <v>1</v>
       </c>
       <c r="Q5" t="n">
-        <v>238</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>4769</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -763,44 +763,44 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Robinson_Crusoe.txt</t>
+          <t>Hobbit_en.txt</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>271</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>121082</v>
+        <v>95384</v>
       </c>
       <c r="E6" t="n">
-        <v>6178</v>
+        <v>6483</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9847</v>
+        <v>8.0549</v>
       </c>
       <c r="G6" t="n">
-        <v>1.33429768</v>
+        <v>1.16997457</v>
       </c>
       <c r="H6" t="n">
-        <v>0.55556046</v>
+        <v>0.47023584</v>
       </c>
       <c r="I6" t="n">
-        <v>1.25973662</v>
+        <v>1.25520989</v>
       </c>
       <c r="J6" t="n">
-        <v>0.49050132</v>
+        <v>0.43887481</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6043271099999999</v>
+        <v>0.53799699</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1123994</v>
+        <v>0.08672349</v>
       </c>
       <c r="M6" t="n">
-        <v>0.62067416</v>
+        <v>0.59312309</v>
       </c>
       <c r="N6" t="n">
-        <v>0.11540657</v>
+        <v>0.09987667</v>
       </c>
       <c r="O6" t="n">
         <v>4760</v>
@@ -821,176 +821,524 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>serbian_èá¼Ñ¡« ñ«íá.txt</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>36206</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8743</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.3407</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.00419913</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.37766987</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.12086598</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.29181093</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.52325194</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.07529261</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.56361018</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.09290163</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1800</v>
+      </c>
+      <c r="P7" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>90</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>serbian_èá¼Ñ¡« ñ«íá_space&amp;paragraph.txt</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" t="n">
+        <v>36206</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8743</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.5992</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.00419913</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.37766987</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.12086598</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.29181093</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.52325194</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.07529261</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.56361018</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.09290163</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="P8" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>90</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Clarke, Arthur C - Cradle.txt</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>140001</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10624</v>
+      </c>
+      <c r="F9" t="n">
+        <v>15.2054</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.19409657</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.52401081</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.39561965</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.70131497</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.5254383</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.07935109</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.5714807</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.08531967</v>
+      </c>
+      <c r="O9" t="n">
+        <v>6650</v>
+      </c>
+      <c r="P9" t="n">
+        <v>350</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>350</v>
+      </c>
+      <c r="R9" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Robinson_Crusoe.txt</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>121082</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6178</v>
+      </c>
+      <c r="F10" t="n">
+        <v>9.8789</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.20134845</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.50751485</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.29438223</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.52242766</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.53466574</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.08445566</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.5933598</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.11338525</v>
+      </c>
+      <c r="O10" t="n">
+        <v>6040</v>
+      </c>
+      <c r="P10" t="n">
+        <v>302</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>302</v>
+      </c>
+      <c r="R10" t="n">
+        <v>6054</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Don_Quixote06w.txt</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>6</v>
+      </c>
+      <c r="D11" t="n">
+        <v>200005</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10062</v>
+      </c>
+      <c r="F11" t="n">
+        <v>19.9805</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.04728719</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.3525048</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.18084668</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.30962379</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.49062637</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.05842974</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.50879319</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.06181332</v>
+      </c>
+      <c r="O11" t="n">
+        <v>9500</v>
+      </c>
+      <c r="P11" t="n">
+        <v>500</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>500</v>
+      </c>
+      <c r="R11" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>+monkey_text_M5k_L1kk.txt</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>153795</v>
+      </c>
+      <c r="E12" t="n">
+        <v>124250</v>
+      </c>
+      <c r="F12" t="n">
+        <v>20.6441</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.8508483999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.23469727</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.86776162</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.22736702</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.47971066</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.05735548</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.479653</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.05750032</v>
+      </c>
+      <c r="O12" t="n">
+        <v>7680</v>
+      </c>
+      <c r="P12" t="n">
+        <v>384</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>384</v>
+      </c>
+      <c r="R12" t="n">
+        <v>7689</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>LOTR_en.txt</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>999</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+      <c r="D13" t="n">
         <v>479149</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E13" t="n">
         <v>14261</v>
       </c>
-      <c r="F7" t="n">
-        <v>11.5258</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.45826326</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.7575868</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.34609843</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.56788795</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.64633531</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.06872863</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.67395573</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.06595175</v>
-      </c>
-      <c r="O7" t="n">
-        <v>4760</v>
-      </c>
-      <c r="P7" t="n">
-        <v>238</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>238</v>
-      </c>
-      <c r="R7" t="n">
-        <v>4769</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="F13" t="n">
+        <v>79.048</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.3914045</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.66834499</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.43428434</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.72912395</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.55759665</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0882106</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.61868786</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.08687661000000001</v>
+      </c>
+      <c r="O13" t="n">
+        <v>23940</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1197</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1197</v>
+      </c>
+      <c r="R13" t="n">
+        <v>23957</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>388.33333333</v>
-      </c>
-      <c r="D8" t="n">
-        <v>178637.83333333</v>
-      </c>
-      <c r="E8" t="n">
-        <v>9391.83333333</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2.89946667</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1.35875214</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.52440937</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1.27877645</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.44186993</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.57925038</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.08629750999999999</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.6012809</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.09315695</v>
-      </c>
-      <c r="O8" t="n">
-        <v>4760</v>
-      </c>
-      <c r="P8" t="n">
-        <v>238</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>238</v>
-      </c>
-      <c r="R8" t="n">
-        <v>4769</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>111139.66666667</v>
+      </c>
+      <c r="E14" t="n">
+        <v>17044.66666667</v>
+      </c>
+      <c r="F14" t="n">
+        <v>14.04383333</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.0063931</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.39942089</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.13122924</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.39829955</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.48088175</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.07095035</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.52236278</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.0827765</v>
+      </c>
+      <c r="O14" t="n">
+        <v>5478.25</v>
+      </c>
+      <c r="P14" t="n">
+        <v>277.5</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>277.5</v>
+      </c>
+      <c r="R14" t="n">
+        <v>5556.75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>StdDev</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Std. Dev.</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>290.72075185</v>
-      </c>
-      <c r="D9" t="n">
-        <v>143054.19943436</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2735.1771068</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3.89020754</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.12059045</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.23926093</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.10505461</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.20641654</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.04577219</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.02610978</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.05225917</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.03179184</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
+      <c r="C15" t="n">
+        <v>1.41421356</v>
+      </c>
+      <c r="D15" t="n">
+        <v>126821.80413828</v>
+      </c>
+      <c r="E15" t="n">
+        <v>32530.74146694</v>
+      </c>
+      <c r="F15" t="n">
+        <v>20.74472467</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.32974771</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.15887995</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.38022248</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.1964753</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.14671977</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.02426944</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.16380581</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.03038015</v>
+      </c>
+      <c r="O15" t="n">
+        <v>6304.92336888</v>
+      </c>
+      <c r="P15" t="n">
+        <v>316.90469125</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>316.90469125</v>
+      </c>
+      <c r="R15" t="n">
+        <v>6340.99686071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>